<commit_message>
Transform PAT table fields to construct event JSON
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Timeline.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F1A528-8741-CA46-BA49-F580B49F196B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C55E659-8E44-FD4C-B1B2-A2A2B74B0058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>table_name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>dict</t>
   </si>
   <si>
-    <t>table</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -175,12 +172,6 @@
   </si>
   <si>
     <t>Opg\Core\Model\Event\Common\NoteCreated</t>
-  </si>
-  <si>
-    <t>Case is already present because of the generate_timeline_event_data transform</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>Derived from Title, Forename, Surname, Case in the transform
@@ -205,6 +196,9 @@
   </si>
   <si>
     <t>Stub column so insert statements are constructed correctly; if there are no mappings which include a casrec table name, it's not set, and the insert statements break</t>
+  </si>
+  <si>
+    <t>Case, Title, Forename, Surname</t>
   </si>
 </sst>
 </file>
@@ -518,7 +512,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -536,31 +530,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -574,15 +565,15 @@
         <v>25</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10" t="s">
-        <v>51</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
@@ -595,7 +586,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="10"/>
       <c r="H3" s="10"/>
@@ -616,89 +607,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="67.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="131.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="131.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
@@ -707,825 +696,806 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="b">
+      <c r="E2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="4" t="b">
+      <c r="E3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="7">
+      <c r="M3" s="7">
         <v>2657</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="b">
+      <c r="E4" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="4" t="b">
+      <c r="E5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="225" x14ac:dyDescent="0.2">
+      <c r="L5" s="4"/>
+      <c r="M5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="211" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="4" t="b">
+      <c r="E6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="N6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="9"/>
+      <c r="M6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="3" t="b">
+      <c r="E7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q7" s="3" t="s">
+      <c r="H7" t="s">
         <v>38</v>
       </c>
-      <c r="R7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="5"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="5"/>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="5"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="5"/>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C48" s="5"/>
-    </row>
-    <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C49" s="5"/>
-    </row>
-    <row r="50" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C52" s="5"/>
-    </row>
-    <row r="53" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C53" s="5"/>
-    </row>
-    <row r="54" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C54" s="5"/>
-    </row>
-    <row r="55" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C55" s="5"/>
-    </row>
-    <row r="56" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C56" s="5"/>
-    </row>
-    <row r="57" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C57" s="5"/>
-    </row>
-    <row r="58" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C58" s="5"/>
-    </row>
-    <row r="59" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C59" s="5"/>
-    </row>
-    <row r="60" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C60" s="5"/>
-    </row>
-    <row r="61" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C64" s="5"/>
-    </row>
-    <row r="65" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C66" s="5"/>
-    </row>
-    <row r="67" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C68" s="5"/>
-    </row>
-    <row r="69" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C69" s="5"/>
-    </row>
-    <row r="70" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C70" s="5"/>
-    </row>
-    <row r="71" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C71" s="5"/>
-    </row>
-    <row r="72" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C72" s="5"/>
-    </row>
-    <row r="73" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C73" s="5"/>
-    </row>
-    <row r="74" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C74" s="5"/>
-    </row>
-    <row r="75" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C77" s="5"/>
-    </row>
-    <row r="78" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C81" s="5"/>
-    </row>
-    <row r="82" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C86" s="5"/>
-    </row>
-    <row r="87" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C87" s="5"/>
-    </row>
-    <row r="88" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C88" s="5"/>
-    </row>
-    <row r="89" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C89" s="5"/>
-    </row>
-    <row r="90" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C90" s="5"/>
-    </row>
-    <row r="91" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C91" s="5"/>
-    </row>
-    <row r="92" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C92" s="5"/>
-    </row>
-    <row r="93" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C93" s="5"/>
-    </row>
-    <row r="94" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C94" s="5"/>
-    </row>
-    <row r="95" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C95" s="5"/>
-    </row>
-    <row r="96" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C96" s="5"/>
-    </row>
-    <row r="97" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C97" s="5"/>
-    </row>
-    <row r="98" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C98" s="5"/>
-    </row>
-    <row r="99" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C99" s="5"/>
-    </row>
-    <row r="100" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C100" s="5"/>
-    </row>
-    <row r="101" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C101" s="5"/>
-    </row>
-    <row r="102" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C102" s="5"/>
-    </row>
-    <row r="103" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C103" s="5"/>
-    </row>
-    <row r="104" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C104" s="5"/>
-    </row>
-    <row r="105" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C105" s="5"/>
-    </row>
-    <row r="106" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C106" s="5"/>
-    </row>
-    <row r="107" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C107" s="5"/>
-    </row>
-    <row r="108" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C108" s="5"/>
-    </row>
-    <row r="109" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C109" s="5"/>
-    </row>
-    <row r="110" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C110" s="5"/>
-    </row>
-    <row r="111" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C111" s="5"/>
-    </row>
-    <row r="112" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C112" s="5"/>
-    </row>
-    <row r="113" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C113" s="5"/>
-    </row>
-    <row r="114" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C114" s="5"/>
-    </row>
-    <row r="115" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C115" s="5"/>
-    </row>
-    <row r="116" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C116" s="5"/>
-    </row>
-    <row r="117" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C117" s="5"/>
-    </row>
-    <row r="118" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C118" s="5"/>
-    </row>
-    <row r="119" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C119" s="5"/>
-    </row>
-    <row r="120" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C120" s="5"/>
-    </row>
-    <row r="121" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C121" s="5"/>
-    </row>
-    <row r="122" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C122" s="5"/>
-    </row>
-    <row r="123" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C123" s="5"/>
-    </row>
-    <row r="124" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C124" s="5"/>
-    </row>
-    <row r="125" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C125" s="5"/>
-    </row>
-    <row r="126" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C126" s="5"/>
-    </row>
-    <row r="127" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C127" s="5"/>
-    </row>
-    <row r="128" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C128" s="5"/>
-    </row>
-    <row r="129" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C129" s="5"/>
-    </row>
-    <row r="130" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C130" s="5"/>
-    </row>
-    <row r="131" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C131" s="5"/>
-    </row>
-    <row r="132" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C132" s="5"/>
-    </row>
-    <row r="133" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C133" s="5"/>
-    </row>
-    <row r="134" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C134" s="5"/>
-    </row>
-    <row r="135" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C135" s="5"/>
-    </row>
-    <row r="136" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C136" s="5"/>
-    </row>
-    <row r="137" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C137" s="5"/>
-    </row>
-    <row r="138" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C138" s="5"/>
-    </row>
-    <row r="139" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C139" s="5"/>
-    </row>
-    <row r="140" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C140" s="5"/>
-    </row>
-    <row r="141" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C141" s="5"/>
-    </row>
-    <row r="142" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C142" s="5"/>
-    </row>
-    <row r="143" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C143" s="5"/>
-    </row>
-    <row r="144" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C144" s="5"/>
-    </row>
-    <row r="145" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C145" s="5"/>
-    </row>
-    <row r="146" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C146" s="5"/>
-    </row>
-    <row r="147" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C147" s="5"/>
-    </row>
-    <row r="148" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C148" s="5"/>
-    </row>
-    <row r="149" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C149" s="5"/>
-    </row>
-    <row r="150" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C150" s="5"/>
-    </row>
-    <row r="151" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C151" s="5"/>
-    </row>
-    <row r="152" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C152" s="5"/>
-    </row>
-    <row r="153" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C153" s="5"/>
-    </row>
-    <row r="154" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C154" s="5"/>
-    </row>
-    <row r="155" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C155" s="5"/>
-    </row>
-    <row r="156" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C156" s="5"/>
-    </row>
-    <row r="157" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C157" s="5"/>
-    </row>
-    <row r="158" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C158" s="5"/>
-    </row>
-    <row r="159" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C159" s="5"/>
-    </row>
-    <row r="160" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C160" s="5"/>
-    </row>
-    <row r="161" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C161" s="5"/>
-    </row>
-    <row r="162" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C162" s="5"/>
-    </row>
-    <row r="163" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C163" s="5"/>
-    </row>
-    <row r="164" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C164" s="5"/>
-    </row>
-    <row r="165" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C165" s="5"/>
-    </row>
-    <row r="166" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C166" s="5"/>
-    </row>
-    <row r="167" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C167" s="5"/>
-    </row>
-    <row r="168" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C168" s="5"/>
-    </row>
-    <row r="169" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C169" s="5"/>
-    </row>
-    <row r="170" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C170" s="5"/>
-    </row>
-    <row r="171" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C171" s="5"/>
-    </row>
-    <row r="172" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C172" s="5"/>
-    </row>
-    <row r="173" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C173" s="5"/>
-    </row>
-    <row r="174" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C174" s="5"/>
-    </row>
-    <row r="175" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C175" s="5"/>
-    </row>
-    <row r="176" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C176" s="5"/>
-    </row>
-    <row r="177" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C177" s="5"/>
-    </row>
-    <row r="178" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C178" s="5"/>
-    </row>
-    <row r="179" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C179" s="5"/>
-    </row>
-    <row r="180" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C180" s="5"/>
-    </row>
-    <row r="181" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C181" s="5"/>
-    </row>
-    <row r="182" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C182" s="5"/>
-    </row>
-    <row r="183" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C183" s="5"/>
-    </row>
-    <row r="184" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C184" s="5"/>
-    </row>
-    <row r="185" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C185" s="5"/>
-    </row>
-    <row r="186" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C186" s="5"/>
-    </row>
-    <row r="187" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C187" s="5"/>
-    </row>
-    <row r="188" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C188" s="5"/>
-    </row>
-    <row r="189" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C189" s="5"/>
-    </row>
-    <row r="190" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C190" s="5"/>
-    </row>
-    <row r="191" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C191" s="5"/>
-    </row>
-    <row r="192" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C192" s="5"/>
-    </row>
-    <row r="193" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C193" s="5"/>
-    </row>
-    <row r="194" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C194" s="5"/>
-    </row>
-    <row r="195" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C195" s="5"/>
-    </row>
-    <row r="196" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C196" s="5"/>
-    </row>
-    <row r="197" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C197" s="5"/>
-    </row>
-    <row r="198" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C198" s="5"/>
-    </row>
-    <row r="199" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C199" s="5"/>
-    </row>
-    <row r="200" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C200" s="5"/>
-    </row>
-    <row r="201" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C201" s="5"/>
-    </row>
-    <row r="202" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C202" s="5"/>
-    </row>
-    <row r="203" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C203" s="5"/>
-    </row>
-    <row r="204" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C204" s="5"/>
-    </row>
-    <row r="205" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C205" s="5"/>
-    </row>
-    <row r="206" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C206" s="5"/>
-    </row>
-    <row r="207" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C207" s="5"/>
-    </row>
-    <row r="208" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C208" s="5"/>
-    </row>
-    <row r="209" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C209" s="5"/>
-    </row>
-    <row r="210" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C210" s="5"/>
-    </row>
-    <row r="211" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C211" s="5"/>
-    </row>
-    <row r="212" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C212" s="5"/>
-    </row>
-    <row r="213" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C213" s="5"/>
-    </row>
-    <row r="214" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C214" s="5"/>
-    </row>
-    <row r="215" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C215" s="5"/>
-    </row>
-    <row r="216" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C216" s="5"/>
-    </row>
-    <row r="217" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C217" s="5"/>
-    </row>
-    <row r="218" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C218" s="5"/>
-    </row>
-    <row r="219" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C219" s="5"/>
-    </row>
-    <row r="220" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C220" s="5"/>
-    </row>
-    <row r="221" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="J7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B50" s="5"/>
+    </row>
+    <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B53" s="5"/>
+    </row>
+    <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B70" s="5"/>
+    </row>
+    <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B73" s="5"/>
+    </row>
+    <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B74" s="5"/>
+    </row>
+    <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B75" s="5"/>
+    </row>
+    <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B76" s="5"/>
+    </row>
+    <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B77" s="5"/>
+    </row>
+    <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B78" s="5"/>
+    </row>
+    <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B79" s="5"/>
+    </row>
+    <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B82" s="5"/>
+    </row>
+    <row r="83" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B83" s="5"/>
+    </row>
+    <row r="84" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B84" s="5"/>
+    </row>
+    <row r="85" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B85" s="5"/>
+    </row>
+    <row r="86" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B86" s="5"/>
+    </row>
+    <row r="87" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B87" s="5"/>
+    </row>
+    <row r="88" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B89" s="5"/>
+    </row>
+    <row r="90" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B90" s="5"/>
+    </row>
+    <row r="91" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B91" s="5"/>
+    </row>
+    <row r="92" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B93" s="5"/>
+    </row>
+    <row r="94" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B94" s="5"/>
+    </row>
+    <row r="95" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B95" s="5"/>
+    </row>
+    <row r="96" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B96" s="5"/>
+    </row>
+    <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B97" s="5"/>
+    </row>
+    <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B100" s="5"/>
+    </row>
+    <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B104" s="5"/>
+    </row>
+    <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B105" s="5"/>
+    </row>
+    <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B106" s="5"/>
+    </row>
+    <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B108" s="5"/>
+    </row>
+    <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B109" s="5"/>
+    </row>
+    <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B110" s="5"/>
+    </row>
+    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B112" s="5"/>
+    </row>
+    <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B113" s="5"/>
+    </row>
+    <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B114" s="5"/>
+    </row>
+    <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B115" s="5"/>
+    </row>
+    <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B116" s="5"/>
+    </row>
+    <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B117" s="5"/>
+    </row>
+    <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B118" s="5"/>
+    </row>
+    <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B119" s="5"/>
+    </row>
+    <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B120" s="5"/>
+    </row>
+    <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B121" s="5"/>
+    </row>
+    <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B122" s="5"/>
+    </row>
+    <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B123" s="5"/>
+    </row>
+    <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B125" s="5"/>
+    </row>
+    <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B126" s="5"/>
+    </row>
+    <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B127" s="5"/>
+    </row>
+    <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B128" s="5"/>
+    </row>
+    <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B129" s="5"/>
+    </row>
+    <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B130" s="5"/>
+    </row>
+    <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B131" s="5"/>
+    </row>
+    <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B132" s="5"/>
+    </row>
+    <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B133" s="5"/>
+    </row>
+    <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B134" s="5"/>
+    </row>
+    <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B135" s="5"/>
+    </row>
+    <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B136" s="5"/>
+    </row>
+    <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B137" s="5"/>
+    </row>
+    <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B138" s="5"/>
+    </row>
+    <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B139" s="5"/>
+    </row>
+    <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B140" s="5"/>
+    </row>
+    <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B141" s="5"/>
+    </row>
+    <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B142" s="5"/>
+    </row>
+    <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B143" s="5"/>
+    </row>
+    <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B144" s="5"/>
+    </row>
+    <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B145" s="5"/>
+    </row>
+    <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B146" s="5"/>
+    </row>
+    <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B147" s="5"/>
+    </row>
+    <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B148" s="5"/>
+    </row>
+    <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B149" s="5"/>
+    </row>
+    <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B150" s="5"/>
+    </row>
+    <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B151" s="5"/>
+    </row>
+    <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B152" s="5"/>
+    </row>
+    <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B153" s="5"/>
+    </row>
+    <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B154" s="5"/>
+    </row>
+    <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B155" s="5"/>
+    </row>
+    <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B156" s="5"/>
+    </row>
+    <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B157" s="5"/>
+    </row>
+    <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B158" s="5"/>
+    </row>
+    <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B159" s="5"/>
+    </row>
+    <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B160" s="5"/>
+    </row>
+    <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B161" s="5"/>
+    </row>
+    <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B162" s="5"/>
+    </row>
+    <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B163" s="5"/>
+    </row>
+    <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B164" s="5"/>
+    </row>
+    <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B165" s="5"/>
+    </row>
+    <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B166" s="5"/>
+    </row>
+    <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B167" s="5"/>
+    </row>
+    <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B168" s="5"/>
+    </row>
+    <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B169" s="5"/>
+    </row>
+    <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B170" s="5"/>
+    </row>
+    <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B171" s="5"/>
+    </row>
+    <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B172" s="5"/>
+    </row>
+    <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B173" s="5"/>
+    </row>
+    <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B174" s="5"/>
+    </row>
+    <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B175" s="5"/>
+    </row>
+    <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B176" s="5"/>
+    </row>
+    <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B177" s="5"/>
+    </row>
+    <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B178" s="5"/>
+    </row>
+    <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B179" s="5"/>
+    </row>
+    <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B180" s="5"/>
+    </row>
+    <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B181" s="5"/>
+    </row>
+    <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B182" s="5"/>
+    </row>
+    <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B183" s="5"/>
+    </row>
+    <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B184" s="5"/>
+    </row>
+    <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B185" s="5"/>
+    </row>
+    <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B186" s="5"/>
+    </row>
+    <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B187" s="5"/>
+    </row>
+    <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B188" s="5"/>
+    </row>
+    <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B189" s="5"/>
+    </row>
+    <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B190" s="5"/>
+    </row>
+    <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B191" s="5"/>
+    </row>
+    <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B192" s="5"/>
+    </row>
+    <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B193" s="5"/>
+    </row>
+    <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B194" s="5"/>
+    </row>
+    <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B195" s="5"/>
+    </row>
+    <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B196" s="5"/>
+    </row>
+    <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B197" s="5"/>
+    </row>
+    <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B198" s="5"/>
+    </row>
+    <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B199" s="5"/>
+    </row>
+    <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B200" s="5"/>
+    </row>
+    <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B201" s="5"/>
+    </row>
+    <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B202" s="5"/>
+    </row>
+    <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B203" s="5"/>
+    </row>
+    <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B204" s="5"/>
+    </row>
+    <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B205" s="5"/>
+    </row>
+    <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B206" s="5"/>
+    </row>
+    <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B207" s="5"/>
+    </row>
+    <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B208" s="5"/>
+    </row>
+    <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B209" s="5"/>
+    </row>
+    <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B210" s="5"/>
+    </row>
+    <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B211" s="5"/>
+    </row>
+    <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B212" s="5"/>
+    </row>
+    <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B213" s="5"/>
+    </row>
+    <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B214" s="5"/>
+    </row>
+    <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B215" s="5"/>
+    </row>
+    <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B216" s="5"/>
+    </row>
+    <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B217" s="5"/>
+    </row>
+    <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B218" s="5"/>
+    </row>
+    <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B219" s="5"/>
+    </row>
+    <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B220" s="5"/>
+    </row>
+    <row r="221" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2312,9 +2282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2417,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2440,7 +2410,7 @@
         <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2463,7 +2433,7 @@
         <v>24</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
IN-1256 create away date event
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Timeline.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C55E659-8E44-FD4C-B1B2-A2A2B74B0058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E6211E-FF3C-6A46-9983-9DB160D5C714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="3" r:id="rId1"/>
@@ -198,7 +198,7 @@
     <t>Stub column so insert statements are constructed correctly; if there are no mappings which include a casrec table name, it's not set, and the insert statements break</t>
   </si>
   <si>
-    <t>Case, Title, Forename, Surname</t>
+    <t>Case, Title, Forename, Surname, Away Date</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95B00FD-C27E-6A43-92F6-E1758A72DC55}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -524,7 +524,7 @@
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" customWidth="1"/>
     <col min="9" max="9" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -611,7 +611,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -850,6 +850,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
       <c r="B8" s="5"/>
       <c r="P8" s="3"/>
     </row>
@@ -2282,7 +2283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>

</xml_diff>

<commit_message>
IN-1256 create away date event (#689)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Timeline.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C55E659-8E44-FD4C-B1B2-A2A2B74B0058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E6211E-FF3C-6A46-9983-9DB160D5C714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="3" r:id="rId1"/>
@@ -198,7 +198,7 @@
     <t>Stub column so insert statements are constructed correctly; if there are no mappings which include a casrec table name, it's not set, and the insert statements break</t>
   </si>
   <si>
-    <t>Case, Title, Forename, Surname</t>
+    <t>Case, Title, Forename, Surname, Away Date</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95B00FD-C27E-6A43-92F6-E1758A72DC55}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -524,7 +524,7 @@
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" customWidth="1"/>
     <col min="9" max="9" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -611,7 +611,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -850,6 +850,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
       <c r="B8" s="5"/>
       <c r="P8" s="3"/>
     </row>
@@ -2282,7 +2283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>

</xml_diff>